<commit_message>
hpw omt updated script
</commit_message>
<xml_diff>
--- a/OMT.xlsx
+++ b/OMT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GoProdScript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prod script\GoProdScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE42F62-D66F-4513-B32D-6C81FBFF3628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="812"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="15" r:id="rId1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="445">
   <si>
     <t>TimeStamp</t>
   </si>
@@ -1295,12 +1296,90 @@
   </si>
   <si>
     <t>OMT_Acqui_FTA_CompletedProd</t>
+  </si>
+  <si>
+    <t>OMT_HPW_CompletedProd</t>
+  </si>
+  <si>
+    <t>Globe At Home Prepaid WiFi</t>
+  </si>
+  <si>
+    <t>₱ 799.00</t>
+  </si>
+  <si>
+    <t>HPW_HappyPath_Completed</t>
+  </si>
+  <si>
+    <t>HPW_TL_PROD</t>
+  </si>
+  <si>
+    <t>HPW_Gots _Agent_PROD</t>
+  </si>
+  <si>
+    <t>HPW_PAL_ Agent_PROD</t>
+  </si>
+  <si>
+    <t>HPW_RSO_ Agent_PROD</t>
+  </si>
+  <si>
+    <t>ms213421</t>
+  </si>
+  <si>
+    <t>anusha</t>
+  </si>
+  <si>
+    <t>ms213425</t>
+  </si>
+  <si>
+    <t>Patra</t>
+  </si>
+  <si>
+    <t>ztie0151</t>
+  </si>
+  <si>
+    <t>Globe@2022</t>
+  </si>
+  <si>
+    <t>francis</t>
+  </si>
+  <si>
+    <t>cashondelivery</t>
+  </si>
+  <si>
+    <t>GLE-000270585</t>
+  </si>
+  <si>
+    <t>2023_01_10_12_01_41</t>
+  </si>
+  <si>
+    <t>CLAIRE ANGELINE VALDEZ DE GUZMAN,shaik.asma@globe.com.ph</t>
+  </si>
+  <si>
+    <t>12,aneex, METRO MANILA , CITY OF PARAÑAQUE , Don Bosco ,1700</t>
+  </si>
+  <si>
+    <t>For Processing</t>
+  </si>
+  <si>
+    <t>2023-01-10 12:01:41</t>
+  </si>
+  <si>
+    <t>2023-01-10_12_01_41</t>
+  </si>
+  <si>
+    <t>VerifyOMTOrder_ForDispatch</t>
+  </si>
+  <si>
+    <t>VerifyOMTOrder_ForActivated</t>
+  </si>
+  <si>
+    <t>OMTValidate_PALAgent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1440,7 +1519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1494,14 +1573,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1509,11 +1582,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1794,47 +1867,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="49.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="49.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="31.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.81640625" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="79.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="28.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="52.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="85.36328125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="28.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="52.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="79.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="79.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="52.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="42.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="79.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="21.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="79.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="22.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="19.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="60.90625" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="42.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="14" customFormat="1">
@@ -1848,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>269</v>
+        <v>441</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>24</v>
@@ -1857,16 +1930,16 @@
         <v>239</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>268</v>
+        <v>435</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>3</v>
+        <v>439</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>262</v>
@@ -1875,10 +1948,10 @@
         <v>263</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>8</v>
+        <v>440</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>264</v>
@@ -1890,22 +1963,22 @@
         <v>266</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="W1" s="15" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="X1" s="12" t="s">
         <v>18</v>
@@ -1935,7 +2008,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="14" customFormat="1" ht="15.75">
+    <row r="2" spans="1:32" s="14" customFormat="1" ht="15.5">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -1966,7 +2039,7 @@
       <c r="J2" s="13">
         <v>9171194728</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="16" t="s">
         <v>412</v>
       </c>
       <c r="L2" s="13" t="s">
@@ -1978,7 +2051,7 @@
       <c r="N2" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="O2" s="27" t="s">
+      <c r="O2" s="13" t="s">
         <v>413</v>
       </c>
       <c r="P2" s="26" t="s">
@@ -2014,10 +2087,10 @@
       <c r="Z2" s="25" t="s">
         <v>414</v>
       </c>
-      <c r="AA2" s="27" t="s">
+      <c r="AA2" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="AB2" s="28" t="s">
+      <c r="AB2" s="27" t="s">
         <v>38</v>
       </c>
       <c r="AC2" s="26" t="s">
@@ -2031,41 +2104,105 @@
       </c>
       <c r="AF2" s="13"/>
     </row>
-    <row r="3" spans="1:32" s="14" customFormat="1" ht="15.75">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="13"/>
-      <c r="AE3" s="22"/>
-      <c r="AF3" s="13"/>
-    </row>
-    <row r="4" spans="1:32" s="14" customFormat="1" ht="15.75">
+    <row r="3" spans="1:32" s="14" customFormat="1" ht="15.5">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="F3" s="13">
+        <v>7</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="L3" s="13">
+        <v>1</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="AA3" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="AB3" s="27">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="AF3" s="13">
+        <v>9171163173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" s="14" customFormat="1" ht="15.5">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -2076,11 +2213,11 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
-      <c r="K4" s="29"/>
+      <c r="K4" s="16"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
-      <c r="O4" s="27"/>
+      <c r="O4" s="13"/>
       <c r="P4" s="26"/>
       <c r="Q4" s="24"/>
       <c r="R4" s="13"/>
@@ -2092,14 +2229,14 @@
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
       <c r="Z4" s="25"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="28"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="27"/>
       <c r="AC4" s="26"/>
       <c r="AD4" s="13"/>
       <c r="AE4" s="22"/>
       <c r="AF4" s="13"/>
     </row>
-    <row r="5" spans="1:32" s="14" customFormat="1" ht="15.75">
+    <row r="5" spans="1:32" s="14" customFormat="1" ht="15.5">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -2110,11 +2247,11 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
-      <c r="K5" s="29"/>
+      <c r="K5" s="16"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
-      <c r="O5" s="27"/>
+      <c r="O5" s="13"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="24"/>
       <c r="R5" s="13"/>
@@ -2126,14 +2263,14 @@
       <c r="X5" s="13"/>
       <c r="Y5" s="13"/>
       <c r="Z5" s="25"/>
-      <c r="AA5" s="27"/>
-      <c r="AB5" s="28"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="27"/>
       <c r="AC5" s="26"/>
       <c r="AD5" s="13"/>
       <c r="AE5" s="22"/>
       <c r="AF5" s="13"/>
     </row>
-    <row r="6" spans="1:32" s="14" customFormat="1" ht="15.75">
+    <row r="6" spans="1:32" s="14" customFormat="1" ht="15.5">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -2144,11 +2281,11 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
-      <c r="K6" s="29"/>
+      <c r="K6" s="16"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
-      <c r="O6" s="27"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="24"/>
       <c r="R6" s="13"/>
@@ -2160,14 +2297,14 @@
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
       <c r="Z6" s="25"/>
-      <c r="AA6" s="27"/>
-      <c r="AB6" s="28"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="27"/>
       <c r="AC6" s="26"/>
       <c r="AD6" s="13"/>
       <c r="AE6" s="22"/>
       <c r="AF6" s="13"/>
     </row>
-    <row r="7" spans="1:32" s="14" customFormat="1" ht="15.75">
+    <row r="7" spans="1:32" s="14" customFormat="1" ht="15.5">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -2178,11 +2315,11 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="29"/>
+      <c r="K7" s="16"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
-      <c r="O7" s="27"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="26"/>
       <c r="Q7" s="24"/>
       <c r="R7" s="13"/>
@@ -2194,18 +2331,18 @@
       <c r="X7" s="13"/>
       <c r="Y7" s="13"/>
       <c r="Z7" s="25"/>
-      <c r="AA7" s="27"/>
-      <c r="AB7" s="28"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="27"/>
       <c r="AC7" s="26"/>
       <c r="AD7" s="13"/>
       <c r="AE7" s="22"/>
       <c r="AF7" s="13"/>
     </row>
     <row r="8" spans="1:32">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -2231,15 +2368,15 @@
       <c r="AA8" s="13"/>
       <c r="AB8" s="13"/>
       <c r="AC8" s="13"/>
-      <c r="AD8" s="30"/>
-      <c r="AE8" s="27"/>
+      <c r="AD8" s="28"/>
+      <c r="AE8" s="13"/>
       <c r="AF8" s="5"/>
     </row>
     <row r="9" spans="1:32">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -2265,15 +2402,15 @@
       <c r="AA9" s="13"/>
       <c r="AB9" s="13"/>
       <c r="AC9" s="13"/>
-      <c r="AD9" s="31"/>
-      <c r="AE9" s="27"/>
+      <c r="AD9" s="29"/>
+      <c r="AE9" s="13"/>
       <c r="AF9" s="5"/>
     </row>
     <row r="10" spans="1:32">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -2284,7 +2421,7 @@
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
-      <c r="O10" s="27"/>
+      <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="13"/>
@@ -2296,18 +2433,18 @@
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
-      <c r="AA10" s="27"/>
+      <c r="AA10" s="13"/>
       <c r="AB10" s="13"/>
       <c r="AC10" s="13"/>
-      <c r="AD10" s="31"/>
-      <c r="AE10" s="27"/>
+      <c r="AD10" s="29"/>
+      <c r="AE10" s="13"/>
       <c r="AF10" s="5"/>
     </row>
     <row r="11" spans="1:32">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -2318,7 +2455,7 @@
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
-      <c r="O11" s="27"/>
+      <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
@@ -2330,18 +2467,18 @@
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
       <c r="Z11" s="13"/>
-      <c r="AA11" s="27"/>
+      <c r="AA11" s="13"/>
       <c r="AB11" s="13"/>
       <c r="AC11" s="13"/>
-      <c r="AD11" s="31"/>
-      <c r="AE11" s="27"/>
+      <c r="AD11" s="29"/>
+      <c r="AE11" s="13"/>
       <c r="AF11" s="5"/>
     </row>
     <row r="12" spans="1:32">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -2352,11 +2489,11 @@
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
-      <c r="O12" s="27"/>
+      <c r="O12" s="13"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="13"/>
-      <c r="S12" s="31"/>
+      <c r="S12" s="29"/>
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
       <c r="V12" s="13"/>
@@ -2364,14 +2501,14 @@
       <c r="X12" s="13"/>
       <c r="Y12" s="13"/>
       <c r="Z12" s="13"/>
-      <c r="AA12" s="27"/>
+      <c r="AA12" s="13"/>
       <c r="AB12" s="13"/>
       <c r="AC12" s="13"/>
-      <c r="AD12" s="31"/>
-      <c r="AE12" s="27"/>
+      <c r="AD12" s="29"/>
+      <c r="AE12" s="13"/>
       <c r="AF12" s="5"/>
     </row>
-    <row r="13" spans="1:32" s="14" customFormat="1" ht="15.75">
+    <row r="13" spans="1:32" s="14" customFormat="1" ht="15.5">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -2382,11 +2519,11 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
-      <c r="K13" s="29"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
-      <c r="O13" s="27"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="24"/>
       <c r="R13" s="13"/>
@@ -2398,8 +2535,8 @@
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
       <c r="Z13" s="24"/>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="28"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="27"/>
       <c r="AC13" s="26"/>
       <c r="AD13" s="13"/>
       <c r="AE13" s="22"/>
@@ -2412,21 +2549,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="5.1796875" style="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2449,7 +2586,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:6" ht="29">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -2465,7 +2602,7 @@
       <c r="E2" s="21" t="s">
         <v>375</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="5" t="s">
         <v>376</v>
       </c>
     </row>
@@ -2611,19 +2748,19 @@
       <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="5" t="s">
         <v>343</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>408</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="5" t="s">
         <v>344</v>
       </c>
     </row>
@@ -2631,10 +2768,10 @@
       <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="5" t="s">
         <v>373</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -2643,7 +2780,7 @@
       <c r="E11" s="21" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="5" t="s">
         <v>351</v>
       </c>
     </row>
@@ -2651,10 +2788,10 @@
       <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="5" t="s">
         <v>373</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -2671,19 +2808,19 @@
       <c r="A13" s="13">
         <v>12</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="5" t="s">
         <v>377</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>378</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="5" t="s">
         <v>379</v>
       </c>
     </row>
@@ -2691,19 +2828,19 @@
       <c r="A14" s="13">
         <v>13</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="30" t="s">
         <v>382</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="5" t="s">
         <v>383</v>
       </c>
     </row>
@@ -2827,118 +2964,184 @@
         <v>398</v>
       </c>
     </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="14">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D21" t="s">
+        <v>431</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>432</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="14">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>424</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D22" t="s">
+        <v>427</v>
+      </c>
+      <c r="F22" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="14">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>425</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D23" t="s">
+        <v>429</v>
+      </c>
+      <c r="F23" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="14">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>426</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="E7" r:id="rId4"/>
-    <hyperlink ref="E13" r:id="rId5"/>
-    <hyperlink ref="E10" r:id="rId6"/>
-    <hyperlink ref="E2" r:id="rId7"/>
-    <hyperlink ref="E8" r:id="rId8"/>
-    <hyperlink ref="E12" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E10" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E2" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E21" r:id="rId11" xr:uid="{39A0F6E6-7FA3-47AD-A4E5-255C9504C161}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:BF3"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="N1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="39.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="32.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="37.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="39.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="39.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="41.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="37.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="18.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="33.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="18.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="26.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="21.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="33.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="21.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="29.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="21.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="33.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="21.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="5.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.453125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="39.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="32.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="37.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="39.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="39.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="41.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="20.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="37.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="18.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="33.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="18.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="26.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="21.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="33.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="21.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="29.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="21.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="33.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="21.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="33" max="33" width="29" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="21.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="41.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="21.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="28.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="18.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="27.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="18.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="21.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="41.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="21.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="28.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="18.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="27.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="18.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="41" max="41" width="29" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="42" max="42" width="17" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="27.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="14.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="28.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="27.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="27.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="14.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="28.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="27.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="49" max="49" width="29" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="27.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="26.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="27.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="26.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="27.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="16.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="14.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="27.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="26.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="27.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="26.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="27.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="16.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="14.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="63" max="63" width="26" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="14.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="16.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="25.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="16.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="27.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="73" max="73" width="16.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="74" max="74" width="20.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="10.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="14.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="16.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="25.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="16.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="27.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="16.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="20.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="10.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="76" max="76" width="7" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="77" max="77" width="10.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="10.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="78" max="78" width="7" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="79" max="79" width="10.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="79" max="79" width="10.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="80" max="80" width="7" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="81" max="81" width="10.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="81" max="81" width="10.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="82" max="82" width="7" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="83" max="83" width="10.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="84" max="16384" width="9.140625" style="18" collapsed="1"/>
+    <col min="83" max="83" width="10.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="84" max="16384" width="9.1796875" style="18" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58">
@@ -3121,7 +3324,7 @@
       <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="31" t="s">
         <v>280</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -3284,6 +3487,62 @@
       <c r="BD2" s="19"/>
       <c r="BE2" s="19"/>
       <c r="BF2" s="19"/>
+    </row>
+    <row r="3" spans="1:58">
+      <c r="A3" s="18">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>312</v>
+      </c>
+      <c r="F3" t="s">
+        <v>424</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>442</v>
+      </c>
+      <c r="H3" t="s">
+        <v>424</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>444</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>423</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3292,7 +3551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3300,10 +3559,10 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3329,14 +3588,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -3356,7 +3615,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AC65"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
@@ -3365,35 +3624,35 @@
       <selection pane="topRight" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="95.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="95.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="67.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="28.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="62.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="67.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="28.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="62.453125" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="67.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="67.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="35.42578125" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="67.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="67.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="22.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="19.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="35.453125" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -3479,7 +3738,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="30">
+    <row r="2" spans="1:29" ht="29">
       <c r="A2" t="s">
         <v>249</v>
       </c>
@@ -6059,7 +6318,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="19.5">
+    <row r="63" spans="1:25" ht="19">
       <c r="B63" s="9" t="s">
         <v>273</v>
       </c>
@@ -6067,7 +6326,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="19.5">
+    <row r="64" spans="1:25" ht="19">
       <c r="B64" s="9" t="s">
         <v>274</v>
       </c>
@@ -6075,7 +6334,7 @@
         <v>9271010457</v>
       </c>
     </row>
-    <row r="65" spans="2:3" ht="19.5">
+    <row r="65" spans="2:3" ht="19">
       <c r="B65" s="9" t="s">
         <v>277</v>
       </c>
@@ -6091,7 +6350,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6100,37 +6359,37 @@
       <selection pane="topRight" activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="22" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="95.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="95.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="67.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="28.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="62.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="67.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="28.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="62.453125" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="67.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="67.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="33.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="35.42578125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="67.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="20.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="67.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="33.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="22.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="19.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="35.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
@@ -6364,7 +6623,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="30">
+    <row r="4" spans="1:31" ht="29">
       <c r="A4" t="s">
         <v>250</v>
       </c>
@@ -6448,33 +6707,33 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.7265625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="32" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="39.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -6736,40 +6995,40 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.42578125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="18.42578125" style="18" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.7109375" style="18" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="33.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="29.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.85546875" style="18" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="26.28515625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.5703125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.453125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="18.453125" style="18" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.7265625" style="18" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="33.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="29.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.81640625" style="18" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.26953125" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="27.54296875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="15" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="26" style="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="15" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="25.7109375" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="19.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="27.140625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="19.85546875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="16384" width="9.140625" style="18" collapsed="1"/>
+    <col min="22" max="22" width="25.7265625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="27.1796875" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="19.81640625" style="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="16384" width="9.1796875" style="18" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">

</xml_diff>

<commit_message>
Renewal OMT updated Script
</commit_message>
<xml_diff>
--- a/OMT.xlsx
+++ b/OMT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prod script\GoProdScript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectGoProd\GoProdScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE42F62-D66F-4513-B32D-6C81FBFF3628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532F712D-D6EC-432F-ACF0-82BF0E0E1BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="812" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="15" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="458">
   <si>
     <t>TimeStamp</t>
   </si>
@@ -1374,6 +1374,45 @@
   </si>
   <si>
     <t>OMTValidate_PALAgent</t>
+  </si>
+  <si>
+    <t>OMT_Renewal_CompletedProd</t>
+  </si>
+  <si>
+    <t>2023_01_10_09_02_53</t>
+  </si>
+  <si>
+    <t>GLE-000270460</t>
+  </si>
+  <si>
+    <t>Renewal Completed</t>
+  </si>
+  <si>
+    <t>Tristram Miles Wade,tcoe3clicks@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>,Pioneer St.,,,,,1554</t>
+  </si>
+  <si>
+    <t>GPlan 999 with Device</t>
+  </si>
+  <si>
+    <t>VerifyOMTOrder_ForOrderCreation</t>
+  </si>
+  <si>
+    <t>VerifyOrder_OrderCreated</t>
+  </si>
+  <si>
+    <t>VerifyOMTOrderStatus_ForProcessing</t>
+  </si>
+  <si>
+    <t>VerifyOrder_Delivered</t>
+  </si>
+  <si>
+    <t>VerifyOMTOrderStatus_RenewalCompleted</t>
   </si>
 </sst>
 </file>
@@ -1519,7 +1558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1587,6 +1626,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1870,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2203,37 +2245,99 @@
       </c>
     </row>
     <row r="4" spans="1:32" s="14" customFormat="1" ht="15.5">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="22"/>
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="F4" s="13">
+        <v>11</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="J4" s="13">
+        <v>9171421883</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="33">
+        <v>44936.377002314817</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="V4" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z4" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB4" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC4" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE4" s="22" t="s">
+        <v>445</v>
+      </c>
       <c r="AF4" s="13"/>
     </row>
     <row r="5" spans="1:32" s="14" customFormat="1" ht="15.5">
@@ -2552,8 +2656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2755,13 +2859,13 @@
         <v>373</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>408</v>
+        <v>372</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3036,12 +3140,12 @@
     <hyperlink ref="E6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
     <hyperlink ref="E7" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
     <hyperlink ref="E13" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="E10" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="E2" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="E8" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="E12" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="E21" r:id="rId11" xr:uid="{39A0F6E6-7FA3-47AD-A4E5-255C9504C161}"/>
+    <hyperlink ref="E2" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E12" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E21" r:id="rId10" xr:uid="{39A0F6E6-7FA3-47AD-A4E5-255C9504C161}"/>
+    <hyperlink ref="E10" r:id="rId11" xr:uid="{8888DB0D-D228-4556-B3D1-1D06EB2FA3FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>
@@ -3050,10 +3154,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BF3"/>
+  <dimension ref="A1:BF4"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3544,6 +3648,80 @@
         <v>423</v>
       </c>
     </row>
+    <row r="4" spans="1:58">
+      <c r="A4" s="18">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>445</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>454</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>455</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="P4" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="S4" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="T4" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="U4" s="18" t="s">
+        <v>456</v>
+      </c>
+      <c r="V4" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>457</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>367</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>